<commit_message>
Add test for student_import recruitment_note
</commit_message>
<xml_diff>
--- a/edziennik/tests/test_files/test_1student.xlsx
+++ b/edziennik/tests/test_files/test_1student.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Imię klienta</t>
   </si>
@@ -58,7 +58,10 @@
     <t xml:space="preserve">Nowak</t>
   </si>
   <si>
-    <t xml:space="preserve">Adam</t>
+    <t xml:space="preserve">Olek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ura</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
@@ -185,12 +188,12 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,22 +239,22 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>690506333</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add validation to Student in student_import
</commit_message>
<xml_diff>
--- a/edziennik/tests/test_files/test_1student.xlsx
+++ b/edziennik/tests/test_files/test_1student.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Imię klienta</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">płeć ucznia: f/m (gramatyczne końcówki w automatycznych emailach I smsach)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">język</t>
   </si>
   <si>
     <t xml:space="preserve">grupa</t>
@@ -185,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -224,42 +221,39 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1" t="n">
+        <v>690506333</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>690506333</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="olo@gmail.com"/>
+    <hyperlink ref="H2" r:id="rId1" display="olo@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>